<commit_message>
modify source file and plot
...
</commit_message>
<xml_diff>
--- a/CUDA_Matrix_Addiction/dataSources/time_2070.xlsx
+++ b/CUDA_Matrix_Addiction/dataSources/time_2070.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\UNICAL\MAGISTRALE AIDS\I ANNO\STATISTICA\2021-10-05 markdown and visualization\visualization\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\UNICAL\MAGISTRALE AIDS\I ANNO\GPGPU\GPGPU\CUDA_Matrix_Addiction\dataSources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -469,7 +469,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:I13"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -524,18 +524,19 @@
         <v>12</v>
       </c>
       <c r="D2" s="4">
-        <v>2.7161</v>
+        <f>2.7161*3</f>
+        <v>8.148299999999999</v>
       </c>
       <c r="E2" s="5">
         <v>8.3702000000000005</v>
       </c>
       <c r="F2" s="5">
         <f>Tabella1[[#This Row],[init_min_time]]+Tabella1[[#This Row],[add_min_time]]</f>
-        <v>11.086300000000001</v>
+        <v>16.5185</v>
       </c>
       <c r="G2" s="7">
         <f>1278/Tabella1[[#This Row],[init_min_time]]</f>
-        <v>470.5275947130076</v>
+        <v>156.84253157100255</v>
       </c>
       <c r="H2" s="7">
         <f>294/Tabella1[[#This Row],[add_min_time]]</f>
@@ -543,7 +544,7 @@
       </c>
       <c r="I2" s="7">
         <f>1572/Tabella1[[#This Row],[total_time]]</f>
-        <v>141.79663187898575</v>
+        <v>95.166025970881137</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -557,18 +558,19 @@
         <v>10</v>
       </c>
       <c r="D3" s="4">
-        <v>2.7161</v>
+        <f>2.7161*3</f>
+        <v>8.148299999999999</v>
       </c>
       <c r="E3" s="5">
         <v>8.3836999999999993</v>
       </c>
       <c r="F3" s="5">
         <f>Tabella1[[#This Row],[init_min_time]]+Tabella1[[#This Row],[add_min_time]]</f>
-        <v>11.099799999999998</v>
+        <v>16.531999999999996</v>
       </c>
       <c r="G3" s="7">
         <f>1278/Tabella1[[#This Row],[init_min_time]]</f>
-        <v>470.5275947130076</v>
+        <v>156.84253157100255</v>
       </c>
       <c r="H3" s="7">
         <f>294/Tabella1[[#This Row],[add_min_time]]</f>
@@ -576,7 +578,7 @@
       </c>
       <c r="I3" s="7">
         <f>1572/Tabella1[[#This Row],[total_time]]</f>
-        <v>141.62417340852991</v>
+        <v>95.088313573675322</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -590,18 +592,19 @@
         <v>11</v>
       </c>
       <c r="D4" s="4">
-        <v>3.3245</v>
+        <f>3.3245*3</f>
+        <v>9.9734999999999996</v>
       </c>
       <c r="E4" s="5">
         <v>9.2166999999999994</v>
       </c>
       <c r="F4" s="5">
         <f>Tabella1[[#This Row],[init_min_time]]+Tabella1[[#This Row],[add_min_time]]</f>
-        <v>12.5412</v>
+        <v>19.190199999999997</v>
       </c>
       <c r="G4" s="7">
         <f>1278/Tabella1[[#This Row],[init_min_time]]</f>
-        <v>384.41870958038805</v>
+        <v>128.13956986012934</v>
       </c>
       <c r="H4" s="7">
         <f>294/Tabella1[[#This Row],[add_min_time]]</f>
@@ -609,7 +612,7 @@
       </c>
       <c r="I4" s="7">
         <f>1572/Tabella1[[#This Row],[total_time]]</f>
-        <v>125.34685676011865</v>
+        <v>81.916811705974936</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -623,18 +626,19 @@
         <v>12</v>
       </c>
       <c r="D5" s="4">
-        <v>2.7618999999999998</v>
+        <f>2.7619*3</f>
+        <v>8.2856999999999985</v>
       </c>
       <c r="E5" s="5">
         <v>8.1356000000000002</v>
       </c>
       <c r="F5" s="5">
         <f>Tabella1[[#This Row],[init_min_time]]+Tabella1[[#This Row],[add_min_time]]</f>
-        <v>10.897500000000001</v>
+        <v>16.421299999999999</v>
       </c>
       <c r="G5" s="7">
         <f>1278/Tabella1[[#This Row],[init_min_time]]</f>
-        <v>462.72493573264785</v>
+        <v>154.24164524421596</v>
       </c>
       <c r="H5" s="7">
         <f>294/Tabella1[[#This Row],[add_min_time]]</f>
@@ -642,7 +646,7 @@
       </c>
       <c r="I5" s="7">
         <f>1572/Tabella1[[#This Row],[total_time]]</f>
-        <v>144.25326909841706</v>
+        <v>95.729327154366587</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -656,18 +660,19 @@
         <v>10</v>
       </c>
       <c r="D6" s="4">
-        <v>2.8433999999999999</v>
+        <f>2.8434*3</f>
+        <v>8.5302000000000007</v>
       </c>
       <c r="E6" s="5">
         <v>8.0878999999999994</v>
       </c>
       <c r="F6" s="5">
         <f>Tabella1[[#This Row],[init_min_time]]+Tabella1[[#This Row],[add_min_time]]</f>
-        <v>10.9313</v>
+        <v>16.618099999999998</v>
       </c>
       <c r="G6" s="7">
         <f>1278/Tabella1[[#This Row],[init_min_time]]</f>
-        <v>449.46191179573754</v>
+        <v>149.82063726524581</v>
       </c>
       <c r="H6" s="7">
         <f>294/Tabella1[[#This Row],[add_min_time]]</f>
@@ -675,7 +680,7 @@
       </c>
       <c r="I6" s="7">
         <f>1572/Tabella1[[#This Row],[total_time]]</f>
-        <v>143.8072324426189</v>
+        <v>94.595651729138723</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -689,18 +694,19 @@
         <v>11</v>
       </c>
       <c r="D7" s="4">
-        <v>2.8603000000000001</v>
+        <f>2.8603*3</f>
+        <v>8.5808999999999997</v>
       </c>
       <c r="E7" s="5">
         <v>8.2588000000000008</v>
       </c>
       <c r="F7" s="5">
         <f>Tabella1[[#This Row],[init_min_time]]+Tabella1[[#This Row],[add_min_time]]</f>
-        <v>11.119100000000001</v>
+        <v>16.839700000000001</v>
       </c>
       <c r="G7" s="7">
         <f>1278/Tabella1[[#This Row],[init_min_time]]</f>
-        <v>446.80627906163687</v>
+        <v>148.93542635387897</v>
       </c>
       <c r="H7" s="7">
         <f>294/Tabella1[[#This Row],[add_min_time]]</f>
@@ -708,7 +714,7 @@
       </c>
       <c r="I7" s="7">
         <f>1572/Tabella1[[#This Row],[total_time]]</f>
-        <v>141.37834896709265</v>
+        <v>93.350831665647249</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -722,18 +728,19 @@
         <v>12</v>
       </c>
       <c r="D8" s="4">
-        <v>2.7450999999999999</v>
+        <f>2.7451*3</f>
+        <v>8.2352999999999987</v>
       </c>
       <c r="E8" s="5">
         <v>8.2940000000000005</v>
       </c>
       <c r="F8" s="5">
         <f>Tabella1[[#This Row],[init_min_time]]+Tabella1[[#This Row],[add_min_time]]</f>
-        <v>11.039100000000001</v>
+        <v>16.529299999999999</v>
       </c>
       <c r="G8" s="7">
         <f>1278/Tabella1[[#This Row],[init_min_time]]</f>
-        <v>465.55681031656405</v>
+        <v>155.18560343885471</v>
       </c>
       <c r="H8" s="7">
         <f>294/Tabella1[[#This Row],[add_min_time]]</f>
@@ -741,7 +748,7 @@
       </c>
       <c r="I8" s="7">
         <f>1572/Tabella1[[#This Row],[total_time]]</f>
-        <v>142.40291328097396</v>
+        <v>95.103845897890423</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -755,18 +762,19 @@
         <v>10</v>
       </c>
       <c r="D9" s="4">
-        <v>2.8815</v>
+        <f>2.8815*3</f>
+        <v>8.6445000000000007</v>
       </c>
       <c r="E9" s="6">
         <v>8.0569000000000006</v>
       </c>
       <c r="F9" s="5">
         <f>Tabella1[[#This Row],[init_min_time]]+Tabella1[[#This Row],[add_min_time]]</f>
-        <v>10.938400000000001</v>
+        <v>16.7014</v>
       </c>
       <c r="G9" s="7">
         <f>1278/Tabella1[[#This Row],[init_min_time]]</f>
-        <v>443.5190005205622</v>
+        <v>147.83966684018739</v>
       </c>
       <c r="H9" s="7">
         <f>294/Tabella1[[#This Row],[add_min_time]]</f>
@@ -774,7 +782,7 @@
       </c>
       <c r="I9" s="7">
         <f>1572/Tabella1[[#This Row],[total_time]]</f>
-        <v>143.71388868573098</v>
+        <v>94.123845905133706</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -788,18 +796,19 @@
         <v>11</v>
       </c>
       <c r="D10" s="4">
-        <v>3.5874000000000001</v>
+        <f>3.5874*3</f>
+        <v>10.7622</v>
       </c>
       <c r="E10" s="5">
         <v>9.8440999999999992</v>
       </c>
       <c r="F10" s="5">
         <f>Tabella1[[#This Row],[init_min_time]]+Tabella1[[#This Row],[add_min_time]]</f>
-        <v>13.4315</v>
+        <v>20.606299999999997</v>
       </c>
       <c r="G10" s="7">
         <f>1278/Tabella1[[#This Row],[init_min_time]]</f>
-        <v>356.24686402408429</v>
+        <v>118.74895467469476</v>
       </c>
       <c r="H10" s="7">
         <f>294/Tabella1[[#This Row],[add_min_time]]</f>
@@ -807,7 +816,7 @@
       </c>
       <c r="I10" s="8">
         <f>1572/Tabella1[[#This Row],[total_time]]</f>
-        <v>117.03830547593344</v>
+        <v>76.287349014621753</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -821,18 +830,19 @@
         <v>12</v>
       </c>
       <c r="D11" s="4">
-        <v>2.6909999999999998</v>
+        <f>2.691*3</f>
+        <v>8.0730000000000004</v>
       </c>
       <c r="E11" s="5">
         <v>8.2622</v>
       </c>
       <c r="F11" s="5">
         <f>Tabella1[[#This Row],[init_min_time]]+Tabella1[[#This Row],[add_min_time]]</f>
-        <v>10.953199999999999</v>
+        <v>16.3352</v>
       </c>
       <c r="G11" s="7">
         <f>1278/Tabella1[[#This Row],[init_min_time]]</f>
-        <v>474.91638795986626</v>
+        <v>158.30546265328874</v>
       </c>
       <c r="H11" s="7">
         <f>294/Tabella1[[#This Row],[add_min_time]]</f>
@@ -840,7 +850,7 @@
       </c>
       <c r="I11" s="7">
         <f>1572/Tabella1[[#This Row],[total_time]]</f>
-        <v>143.51970200489356</v>
+        <v>96.233899799206625</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -854,18 +864,19 @@
         <v>10</v>
       </c>
       <c r="D12" s="4">
-        <v>2.9325000000000001</v>
+        <f>2.9325*3</f>
+        <v>8.7974999999999994</v>
       </c>
       <c r="E12" s="5">
         <v>8.9649999999999999</v>
       </c>
       <c r="F12" s="5">
         <f>Tabella1[[#This Row],[init_min_time]]+Tabella1[[#This Row],[add_min_time]]</f>
-        <v>11.897500000000001</v>
+        <v>17.762499999999999</v>
       </c>
       <c r="G12" s="7">
         <f>1278/Tabella1[[#This Row],[init_min_time]]</f>
-        <v>435.80562659846544</v>
+        <v>145.26854219948851</v>
       </c>
       <c r="H12" s="7">
         <f>294/Tabella1[[#This Row],[add_min_time]]</f>
@@ -873,7 +884,7 @@
       </c>
       <c r="I12" s="7">
         <f>1572/Tabella1[[#This Row],[total_time]]</f>
-        <v>132.12859844505147</v>
+        <v>88.50105559465166</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -887,18 +898,19 @@
         <v>11</v>
       </c>
       <c r="D13" s="4">
-        <v>2.8729</v>
+        <f>2.8729*3</f>
+        <v>8.6187000000000005</v>
       </c>
       <c r="E13" s="5">
         <v>8.0504999999999995</v>
       </c>
       <c r="F13" s="5">
         <f>Tabella1[[#This Row],[init_min_time]]+Tabella1[[#This Row],[add_min_time]]</f>
-        <v>10.923399999999999</v>
+        <v>16.6692</v>
       </c>
       <c r="G13" s="7">
         <f>1278/Tabella1[[#This Row],[init_min_time]]</f>
-        <v>444.84667061157717</v>
+        <v>148.28222353719238</v>
       </c>
       <c r="H13" s="7">
         <f>294/Tabella1[[#This Row],[add_min_time]]</f>
@@ -906,7 +918,7 @@
       </c>
       <c r="I13" s="7">
         <f>1572/Tabella1[[#This Row],[total_time]]</f>
-        <v>143.91123642821833</v>
+        <v>94.305665538838099</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>